<commit_message>
new wallet info json format
</commit_message>
<xml_diff>
--- a/data/token/BTT.xlsx
+++ b/data/token/BTT.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>2024-01-09</t>
+  </si>
+  <si>
+    <t>2024-06-06</t>
+  </si>
+  <si>
+    <t>2024-11-15</t>
   </si>
 </sst>
 </file>
@@ -428,7 +434,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,6 +584,22 @@
         <v>1.06E-06</v>
       </c>
     </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>1.19E-06</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>1.04E-06</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>